<commit_message>
amendments to refer to 2020 and 2019 rather than 2019 and 2018
DRG Price file for 2020 and advanced_LENNON file recieved
</commit_message>
<xml_diff>
--- a/FaresIndexDocumentation/Fares Index Data Dictionary.xlsx
+++ b/FaresIndexDocumentation/Fares Index Data Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10500" tabRatio="914" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10500" tabRatio="914" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -1570,7 +1570,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1591,6 +1590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1897,17 +1897,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>408</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1942,7 +1942,7 @@
       <c r="A3" t="s">
         <v>418</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>76</v>
       </c>
       <c r="C3" t="s">
@@ -1971,7 +1971,7 @@
       <c r="A4" t="s">
         <v>418</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
@@ -2000,7 +2000,7 @@
       <c r="A5" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
@@ -2029,7 +2029,7 @@
       <c r="A6" t="s">
         <v>418</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
@@ -2058,7 +2058,7 @@
       <c r="A7" t="s">
         <v>418</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C7" t="s">
@@ -2087,7 +2087,7 @@
       <c r="A8" t="s">
         <v>418</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
@@ -2116,7 +2116,7 @@
       <c r="A9" t="s">
         <v>418</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C9" t="s">
@@ -2145,7 +2145,7 @@
       <c r="A10" t="s">
         <v>418</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>50</v>
       </c>
       <c r="C10" t="s">
@@ -2174,7 +2174,7 @@
       <c r="A11" t="s">
         <v>418</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>62</v>
       </c>
       <c r="C11" t="s">
@@ -2203,7 +2203,7 @@
       <c r="A12" t="s">
         <v>418</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>65</v>
       </c>
       <c r="C12" t="s">
@@ -2232,7 +2232,7 @@
       <c r="A13" t="s">
         <v>418</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C13" t="s">
@@ -2261,7 +2261,7 @@
       <c r="A14" t="s">
         <v>418</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>66</v>
       </c>
       <c r="C14" t="s">
@@ -2290,7 +2290,7 @@
       <c r="A15" t="s">
         <v>418</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="s">
@@ -2319,7 +2319,7 @@
       <c r="A16" t="s">
         <v>418</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C16" t="s">
@@ -2348,7 +2348,7 @@
       <c r="A17" t="s">
         <v>418</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>72</v>
       </c>
       <c r="C17" t="s">
@@ -2377,7 +2377,7 @@
       <c r="A18" t="s">
         <v>418</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>70</v>
       </c>
       <c r="C18" t="s">
@@ -2406,7 +2406,7 @@
       <c r="A19" t="s">
         <v>418</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>74</v>
       </c>
       <c r="C19" t="s">
@@ -2435,7 +2435,7 @@
       <c r="A20" t="s">
         <v>418</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C20" t="s">
@@ -2464,7 +2464,7 @@
       <c r="A21" t="s">
         <v>418</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>80</v>
       </c>
       <c r="C21" t="s">
@@ -2504,7 +2504,7 @@
       <c r="A23" t="s">
         <v>419</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C23" t="s">
@@ -2533,7 +2533,7 @@
       <c r="A24" t="s">
         <v>419</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C24" t="s">
@@ -2562,7 +2562,7 @@
       <c r="A25" t="s">
         <v>419</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C25" t="s">
@@ -2591,7 +2591,7 @@
       <c r="A26" t="s">
         <v>419</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C26" t="s">
@@ -2620,7 +2620,7 @@
       <c r="A27" t="s">
         <v>419</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C27" t="s">
@@ -2793,7 +2793,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -2804,7 +2804,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3675,7 +3675,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -3686,7 +3686,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -4500,7 +4500,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -4511,7 +4511,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -4610,7 +4610,7 @@
       <c r="F7">
         <v>45487</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="17" t="s">
         <v>257</v>
       </c>
       <c r="H7" t="s">
@@ -4653,7 +4653,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -4664,7 +4664,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -5004,7 +5004,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -5015,7 +5015,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -6639,7 +6639,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -6650,7 +6650,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -6818,7 +6818,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -6829,10 +6829,10 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>361</v>
       </c>
     </row>
@@ -6936,7 +6936,7 @@
       <c r="O3">
         <v>816</v>
       </c>
-      <c r="P3" s="24">
+      <c r="P3" s="23">
         <v>73415</v>
       </c>
     </row>
@@ -6979,7 +6979,7 @@
       <c r="O4">
         <v>875</v>
       </c>
-      <c r="P4" s="24">
+      <c r="P4" s="23">
         <v>73415</v>
       </c>
     </row>
@@ -7022,7 +7022,7 @@
       <c r="O5">
         <v>923</v>
       </c>
-      <c r="P5" s="24">
+      <c r="P5" s="23">
         <v>73415</v>
       </c>
     </row>
@@ -7065,7 +7065,7 @@
       <c r="O6">
         <v>939</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P6" s="23">
         <v>73415</v>
       </c>
     </row>
@@ -7108,7 +7108,7 @@
       <c r="O7">
         <v>853</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7" s="23">
         <v>73415</v>
       </c>
     </row>
@@ -7151,7 +7151,7 @@
       <c r="O8">
         <v>1051</v>
       </c>
-      <c r="P8" s="24">
+      <c r="P8" s="23">
         <v>73415</v>
       </c>
     </row>
@@ -7284,7 +7284,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -7295,7 +7295,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -8211,7 +8211,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -8222,7 +8222,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -9237,7 +9237,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -9248,7 +9248,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -10532,7 +10532,7 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
@@ -10547,7 +10547,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -10623,7 +10623,7 @@
       <c r="K3" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="28">
+      <c r="L3" s="27">
         <v>-36.11</v>
       </c>
       <c r="M3">
@@ -10657,7 +10657,7 @@
       <c r="K4" t="s">
         <v>105</v>
       </c>
-      <c r="L4" s="28">
+      <c r="L4" s="27">
         <v>6.42</v>
       </c>
       <c r="M4">
@@ -10691,7 +10691,7 @@
       <c r="K5" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="27">
         <v>0</v>
       </c>
       <c r="M5">
@@ -10725,7 +10725,7 @@
       <c r="K6" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="27">
         <v>-9.94</v>
       </c>
       <c r="M6">
@@ -10759,7 +10759,7 @@
       <c r="K7" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="27">
         <v>-5.27</v>
       </c>
       <c r="M7">
@@ -10793,7 +10793,7 @@
       <c r="K8" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="27">
         <v>8.4700000000000006</v>
       </c>
       <c r="M8">
@@ -10827,7 +10827,7 @@
       <c r="K9" t="s">
         <v>110</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="27">
         <v>-6.48</v>
       </c>
       <c r="M9">
@@ -10861,7 +10861,7 @@
       <c r="K10" t="s">
         <v>105</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="27">
         <v>5.84</v>
       </c>
       <c r="M10">
@@ -10889,7 +10889,7 @@
       <c r="K11" t="s">
         <v>105</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L11" s="27">
         <v>-5.27</v>
       </c>
       <c r="M11">
@@ -10917,7 +10917,7 @@
       <c r="K12" t="s">
         <v>105</v>
       </c>
-      <c r="L12" s="28">
+      <c r="L12" s="27">
         <v>13.12</v>
       </c>
       <c r="M12">
@@ -10945,7 +10945,7 @@
       <c r="K13" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="27">
         <v>14.6</v>
       </c>
       <c r="M13">
@@ -10973,7 +10973,7 @@
       <c r="K14" t="s">
         <v>103</v>
       </c>
-      <c r="L14" s="28">
+      <c r="L14" s="27">
         <v>0.01</v>
       </c>
       <c r="M14">
@@ -11001,7 +11001,7 @@
       <c r="K15" t="s">
         <v>105</v>
       </c>
-      <c r="L15" s="28">
+      <c r="L15" s="27">
         <v>0.01</v>
       </c>
       <c r="M15">
@@ -11029,7 +11029,7 @@
       <c r="K16" t="s">
         <v>103</v>
       </c>
-      <c r="L16" s="28">
+      <c r="L16" s="27">
         <v>43.66</v>
       </c>
       <c r="M16">
@@ -11057,7 +11057,7 @@
       <c r="K17" t="s">
         <v>103</v>
       </c>
-      <c r="L17" s="28">
+      <c r="L17" s="27">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="M17">
@@ -11085,7 +11085,7 @@
       <c r="K18" t="s">
         <v>103</v>
       </c>
-      <c r="L18" s="28">
+      <c r="L18" s="27">
         <v>6.42</v>
       </c>
       <c r="M18">
@@ -11113,7 +11113,7 @@
       <c r="K19" t="s">
         <v>103</v>
       </c>
-      <c r="L19" s="28">
+      <c r="L19" s="27">
         <v>0.79</v>
       </c>
       <c r="M19">
@@ -11141,7 +11141,7 @@
       <c r="K20" t="s">
         <v>117</v>
       </c>
-      <c r="L20" s="28">
+      <c r="L20" s="27">
         <v>0.11</v>
       </c>
       <c r="M20">
@@ -11169,7 +11169,7 @@
       <c r="K21" t="s">
         <v>117</v>
       </c>
-      <c r="L21" s="28">
+      <c r="L21" s="27">
         <v>0.03</v>
       </c>
       <c r="M21">
@@ -11181,13 +11181,13 @@
       <c r="E22" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="28" t="s">
         <v>428</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
       <c r="F27" t="s">
         <v>85</v>
       </c>
@@ -11243,7 +11243,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -11254,7 +11254,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -11270,47 +11270,47 @@
         <v>206</v>
       </c>
       <c r="E2" s="8"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25" t="s">
+      <c r="L2" s="24"/>
+      <c r="M2" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="24" t="s">
         <v>401</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="P2" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="24" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="A3" s="24"/>
       <c r="B3" t="s">
         <v>255</v>
       </c>
       <c r="C3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="25">
+      <c r="F3" s="24">
         <v>0</v>
       </c>
       <c r="G3" t="s">
@@ -11325,7 +11325,7 @@
       <c r="J3">
         <v>4617868.809999885</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="24">
         <v>0</v>
       </c>
       <c r="M3" t="s">
@@ -11348,7 +11348,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>176</v>
       </c>
       <c r="B4" t="s">
@@ -11356,7 +11356,7 @@
       </c>
       <c r="C4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="25">
+      <c r="F4" s="24">
         <v>1</v>
       </c>
       <c r="G4" t="s">
@@ -11371,7 +11371,7 @@
       <c r="J4">
         <v>242289.75</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="24">
         <v>1</v>
       </c>
       <c r="M4" t="s">
@@ -11394,7 +11394,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>397</v>
       </c>
       <c r="B5" t="s">
@@ -11402,7 +11402,7 @@
       </c>
       <c r="C5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <v>2</v>
       </c>
       <c r="G5" t="s">
@@ -11417,7 +11417,7 @@
       <c r="J5">
         <v>-911091.10000000696</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="24">
         <v>2</v>
       </c>
       <c r="M5" t="s">
@@ -11440,7 +11440,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>398</v>
       </c>
       <c r="B6" t="s">
@@ -11448,7 +11448,7 @@
       </c>
       <c r="C6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <v>3</v>
       </c>
       <c r="G6" t="s">
@@ -11463,7 +11463,7 @@
       <c r="J6">
         <v>24.160000000000011</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="24">
         <v>3</v>
       </c>
       <c r="M6" t="s">
@@ -11486,7 +11486,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>399</v>
       </c>
       <c r="B7" t="s">
@@ -11494,7 +11494,7 @@
       </c>
       <c r="C7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="25">
+      <c r="F7" s="24">
         <v>4</v>
       </c>
       <c r="G7" t="s">
@@ -11509,7 +11509,7 @@
       <c r="J7">
         <v>-62228.319999999992</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="24">
         <v>4</v>
       </c>
       <c r="M7" t="s">
@@ -11534,7 +11534,7 @@
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <v>5</v>
       </c>
       <c r="G8" t="s">
@@ -11549,7 +11549,7 @@
       <c r="J8">
         <v>-62.25</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="24">
         <v>5</v>
       </c>
       <c r="M8" t="s">
@@ -11572,13 +11572,13 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="24"/>
       <c r="B9" t="s">
         <v>255</v>
       </c>
       <c r="C9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <v>6</v>
       </c>
       <c r="G9" t="s">
@@ -11593,7 +11593,7 @@
       <c r="J9">
         <v>35305.979999999872</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="24">
         <v>6</v>
       </c>
       <c r="M9" t="s">
@@ -11616,7 +11616,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>176</v>
       </c>
       <c r="B10" t="s">
@@ -11624,7 +11624,7 @@
       </c>
       <c r="C10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>7</v>
       </c>
       <c r="G10" t="s">
@@ -11639,7 +11639,7 @@
       <c r="J10">
         <v>19763.149999999991</v>
       </c>
-      <c r="L10" s="25">
+      <c r="L10" s="24">
         <v>7</v>
       </c>
       <c r="M10" t="s">
@@ -11662,7 +11662,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>400</v>
       </c>
       <c r="B11" t="s">
@@ -11670,7 +11670,7 @@
       </c>
       <c r="C11" s="8"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="25">
+      <c r="F11" s="24">
         <v>8</v>
       </c>
       <c r="G11" t="s">
@@ -11685,7 +11685,7 @@
       <c r="J11">
         <v>39723.759999999937</v>
       </c>
-      <c r="L11" s="25">
+      <c r="L11" s="24">
         <v>8</v>
       </c>
       <c r="M11" t="s">
@@ -11708,7 +11708,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>401</v>
       </c>
       <c r="B12" t="s">
@@ -11716,7 +11716,7 @@
       </c>
       <c r="C12" s="8"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="25">
+      <c r="F12" s="24">
         <v>9</v>
       </c>
       <c r="G12" t="s">
@@ -11731,7 +11731,7 @@
       <c r="J12">
         <v>2978.380000000001</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="24">
         <v>9</v>
       </c>
       <c r="M12" t="s">
@@ -11754,7 +11754,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>198</v>
       </c>
       <c r="B13" t="s">
@@ -11764,7 +11764,7 @@
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>398</v>
       </c>
       <c r="B14" t="s">
@@ -11774,7 +11774,7 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>399</v>
       </c>
       <c r="B15" t="s">
@@ -11822,7 +11822,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -11833,7 +11833,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -12453,7 +12453,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -12464,7 +12464,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
@@ -12636,7 +12636,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -13091,7 +13091,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -13350,7 +13350,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -13565,7 +13565,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -13816,8 +13816,8 @@
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13838,7 +13838,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -14119,7 +14119,7 @@
       <c r="J10">
         <v>462125</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="29">
         <v>4777</v>
       </c>
       <c r="L10">
@@ -14156,6 +14156,7 @@
     <hyperlink ref="B1" location="'Data Dictionary'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14167,7 +14168,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J3" sqref="J3:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14180,7 +14181,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -14591,7 +14592,7 @@
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>344</v>
       </c>
       <c r="C1" s="8"/>
@@ -14602,7 +14603,7 @@
       <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>267</v>
       </c>
     </row>

</xml_diff>

<commit_message>
error in data catalogue amended
LENNON advanced and non-advance format changed from xlsx to csv
</commit_message>
<xml_diff>
--- a/FaresIndexDocumentation/Fares Index Data Dictionary.xlsx
+++ b/FaresIndexDocumentation/Fares Index Data Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10500" tabRatio="914" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10500" tabRatio="914" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="430">
   <si>
     <t xml:space="preserve">Name of file </t>
   </si>
@@ -1332,6 +1332,9 @@
   </si>
   <si>
     <t>NB: These field names are changed in the code to their previous names:</t>
+  </si>
+  <si>
+    <t>price_YYYY</t>
   </si>
 </sst>
 </file>
@@ -1587,10 +1590,10 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1879,7 +1882,7 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -11181,13 +11184,13 @@
       <c r="E22" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="29" t="s">
         <v>428</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
       <c r="F27" t="s">
         <v>85</v>
       </c>
@@ -13816,8 +13819,8 @@
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13859,7 +13862,7 @@
       </c>
       <c r="C2" s="8"/>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>4</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" t="s">
@@ -14072,7 +14075,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>241</v>
+        <v>429</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -14119,7 +14122,7 @@
       <c r="J10">
         <v>462125</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="28">
         <v>4777</v>
       </c>
       <c r="L10">
@@ -14167,8 +14170,8 @@
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14202,7 +14205,7 @@
       </c>
       <c r="C2" s="8"/>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>4</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" t="s">

</xml_diff>

<commit_message>
env-created for Fares Index
uses Pandas 0.24.0
</commit_message>
<xml_diff>
--- a/FaresIndexDocumentation/Fares Index Data Dictionary.xlsx
+++ b/FaresIndexDocumentation/Fares Index Data Dictionary.xlsx
@@ -14171,7 +14171,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14218,7 +14218,7 @@
         <v>88</v>
       </c>
       <c r="I2" t="s">
-        <v>238</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
         <v>239</v>

</xml_diff>

<commit_message>
removal of df_origin variable
LIkely cause of errors is the LENNON non-advanced lookup info.
</commit_message>
<xml_diff>
--- a/FaresIndexDocumentation/Fares Index Data Dictionary.xlsx
+++ b/FaresIndexDocumentation/Fares Index Data Dictionary.xlsx
@@ -1341,6 +1341,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00000"/>
+  </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1543,7 +1546,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1594,6 +1597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14171,13 +14175,14 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -14248,7 +14253,7 @@
       <c r="I3" t="s">
         <v>243</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="30">
         <v>52.8</v>
       </c>
       <c r="K3">
@@ -14276,7 +14281,7 @@
       <c r="I4" t="s">
         <v>244</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="30">
         <v>40.9</v>
       </c>
       <c r="K4">
@@ -14304,7 +14309,7 @@
       <c r="I5" t="s">
         <v>216</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="30">
         <v>-55.5</v>
       </c>
       <c r="K5">
@@ -14332,7 +14337,7 @@
       <c r="I6" t="s">
         <v>245</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="30">
         <v>2.0299999999999998</v>
       </c>
       <c r="K6">
@@ -14344,7 +14349,7 @@
         <v>239</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>340</v>
       </c>
       <c r="C7" s="8"/>
       <c r="E7" s="8"/>
@@ -14360,7 +14365,7 @@
       <c r="I7" t="s">
         <v>246</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="30">
         <v>64.38</v>
       </c>
       <c r="K7">
@@ -14388,7 +14393,7 @@
       <c r="I8" t="s">
         <v>247</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="30">
         <v>859.53</v>
       </c>
       <c r="K8">
@@ -14410,7 +14415,7 @@
       <c r="I9" t="s">
         <v>248</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="30">
         <v>1.23</v>
       </c>
       <c r="K9">
@@ -14432,7 +14437,7 @@
       <c r="I10" t="s">
         <v>249</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="30">
         <v>1.66</v>
       </c>
       <c r="K10">
@@ -14454,7 +14459,7 @@
       <c r="I11" t="s">
         <v>250</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="30">
         <v>0</v>
       </c>
       <c r="K11">
@@ -14476,7 +14481,7 @@
       <c r="I12" t="s">
         <v>251</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="30">
         <v>5.6</v>
       </c>
       <c r="K12">
@@ -14498,7 +14503,7 @@
       <c r="I13" t="s">
         <v>252</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="30">
         <v>-26.5</v>
       </c>
       <c r="K13">
@@ -14520,7 +14525,7 @@
       <c r="I14" t="s">
         <v>253</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="30">
         <v>133.43</v>
       </c>
       <c r="K14">
@@ -14542,7 +14547,7 @@
       <c r="I15" t="s">
         <v>254</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="30">
         <v>6.33</v>
       </c>
       <c r="K15">
@@ -14554,6 +14559,7 @@
     <hyperlink ref="B1" location="'Data Dictionary'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>